<commit_message>
20170715 - Commit and Push
</commit_message>
<xml_diff>
--- a/Lotto/lotto/lotto-past-draws-archive-2017.xlsx
+++ b/Lotto/lotto/lotto-past-draws-archive-2017.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Lotto</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Bonus Ball</t>
+  </si>
+  <si>
+    <t>12 July 2017</t>
   </si>
   <si>
     <t>08 July 2017</t>
@@ -544,9 +547,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -591,25 +594,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>31</v>
+      </c>
+      <c r="E6">
         <v>33</v>
       </c>
-      <c r="D6">
-        <v>36</v>
-      </c>
-      <c r="E6">
-        <v>38</v>
-      </c>
       <c r="F6">
+        <v>35</v>
+      </c>
+      <c r="G6">
         <v>40</v>
       </c>
-      <c r="G6">
-        <v>45</v>
-      </c>
       <c r="H6">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -617,25 +620,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E7">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F7">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H7">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -643,25 +646,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D8">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E8">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F8">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="G8">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="H8">
-        <v>48</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -669,25 +672,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9">
         <v>25</v>
       </c>
-      <c r="E9">
-        <v>29</v>
-      </c>
-      <c r="F9">
-        <v>30</v>
-      </c>
       <c r="G9">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="H9">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -698,22 +701,22 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F10">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G10">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H10">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -721,25 +724,25 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F11">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="G11">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H11">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -747,25 +750,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E12">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F12">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G12">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H12">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -773,25 +776,25 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E13">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F13">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H13">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -799,25 +802,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E14">
+        <v>19</v>
+      </c>
+      <c r="F14">
+        <v>33</v>
+      </c>
+      <c r="G14">
+        <v>42</v>
+      </c>
+      <c r="H14">
         <v>27</v>
-      </c>
-      <c r="F14">
-        <v>42</v>
-      </c>
-      <c r="G14">
-        <v>47</v>
-      </c>
-      <c r="H14">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -825,25 +828,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15">
+        <v>27</v>
+      </c>
+      <c r="F15">
+        <v>42</v>
+      </c>
+      <c r="G15">
+        <v>47</v>
+      </c>
+      <c r="H15">
         <v>28</v>
-      </c>
-      <c r="F15">
-        <v>32</v>
-      </c>
-      <c r="G15">
-        <v>45</v>
-      </c>
-      <c r="H15">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -851,25 +854,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E16">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F16">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G16">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H16">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -877,25 +880,25 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D17">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E17">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F17">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G17">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -903,25 +906,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C18">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E18">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F18">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G18">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H18">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -929,25 +932,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F19">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G19">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="H19">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -958,22 +961,22 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D20">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E20">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F20">
         <v>30</v>
       </c>
       <c r="G20">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -981,25 +984,25 @@
         <v>19</v>
       </c>
       <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
         <v>12</v>
       </c>
-      <c r="C21">
-        <v>25</v>
-      </c>
-      <c r="D21">
-        <v>27</v>
-      </c>
       <c r="E21">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F21">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G21">
         <v>41</v>
       </c>
       <c r="H21">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1007,25 +1010,25 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E22">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F22">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G22">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H22">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1033,25 +1036,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
         <v>26</v>
       </c>
-      <c r="E23">
-        <v>41</v>
-      </c>
-      <c r="F23">
-        <v>43</v>
-      </c>
       <c r="G23">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H23">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1059,25 +1062,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D24">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E24">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F24">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G24">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H24">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1085,25 +1088,25 @@
         <v>23</v>
       </c>
       <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
         <v>9</v>
       </c>
-      <c r="C25">
-        <v>11</v>
-      </c>
-      <c r="D25">
-        <v>16</v>
-      </c>
       <c r="E25">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F25">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G25">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="H25">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1111,25 +1114,25 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D26">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E26">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F26">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G26">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H26">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1137,25 +1140,25 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D27">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E27">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F27">
+        <v>43</v>
+      </c>
+      <c r="G27">
         <v>47</v>
       </c>
-      <c r="G27">
-        <v>48</v>
-      </c>
       <c r="H27">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1163,25 +1166,25 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D28">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E28">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F28">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G28">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H28">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1189,22 +1192,22 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C29">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D29">
+        <v>23</v>
+      </c>
+      <c r="E29">
         <v>26</v>
       </c>
-      <c r="E29">
-        <v>35</v>
-      </c>
       <c r="F29">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G29">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H29">
         <v>22</v>
@@ -1215,25 +1218,25 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D30">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30">
         <v>35</v>
       </c>
       <c r="F30">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G30">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H30">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1241,25 +1244,25 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C31">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D31">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E31">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F31">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G31">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="H31">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1267,25 +1270,25 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C32">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D32">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E32">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F32">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G32">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1293,25 +1296,25 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C33">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D33">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E33">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F33">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G33">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H33">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1319,25 +1322,25 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C34">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D34">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E34">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F34">
         <v>35</v>
       </c>
       <c r="G34">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1345,25 +1348,25 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D35">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E35">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F35">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G35">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="H35">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1371,25 +1374,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D36">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E36">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F36">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G36">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H36">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1397,25 +1400,25 @@
         <v>35</v>
       </c>
       <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
         <v>5</v>
       </c>
-      <c r="C37">
-        <v>7</v>
-      </c>
       <c r="D37">
+        <v>9</v>
+      </c>
+      <c r="E37">
+        <v>19</v>
+      </c>
+      <c r="F37">
+        <v>24</v>
+      </c>
+      <c r="G37">
+        <v>25</v>
+      </c>
+      <c r="H37">
         <v>17</v>
-      </c>
-      <c r="E37">
-        <v>22</v>
-      </c>
-      <c r="F37">
-        <v>25</v>
-      </c>
-      <c r="G37">
-        <v>35</v>
-      </c>
-      <c r="H37">
-        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1423,25 +1426,25 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E38">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F38">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G38">
+        <v>35</v>
+      </c>
+      <c r="H38">
         <v>49</v>
-      </c>
-      <c r="H38">
-        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1449,25 +1452,25 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>7</v>
+      </c>
+      <c r="E39">
         <v>13</v>
       </c>
-      <c r="D39">
-        <v>14</v>
-      </c>
-      <c r="E39">
-        <v>25</v>
-      </c>
       <c r="F39">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="G39">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="H39">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1475,25 +1478,25 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D40">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E40">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F40">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G40">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1501,25 +1504,25 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C41">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D41">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E41">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F41">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G41">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H41">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1527,25 +1530,25 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C42">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D42">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E42">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F42">
         <v>38</v>
       </c>
       <c r="G42">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H42">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1553,25 +1556,25 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D43">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E43">
+        <v>31</v>
+      </c>
+      <c r="F43">
+        <v>38</v>
+      </c>
+      <c r="G43">
         <v>41</v>
       </c>
-      <c r="F43">
-        <v>43</v>
-      </c>
-      <c r="G43">
-        <v>44</v>
-      </c>
       <c r="H43">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1579,25 +1582,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D44">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="E44">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F44">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G44">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H44">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1608,22 +1611,22 @@
         <v>7</v>
       </c>
       <c r="C45">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D45">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E45">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F45">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G45">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H45">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1631,25 +1634,25 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46">
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>16</v>
+      </c>
+      <c r="E46">
+        <v>39</v>
+      </c>
+      <c r="F46">
+        <v>46</v>
+      </c>
+      <c r="G46">
+        <v>48</v>
+      </c>
+      <c r="H46">
         <v>14</v>
-      </c>
-      <c r="D46">
-        <v>19</v>
-      </c>
-      <c r="E46">
-        <v>31</v>
-      </c>
-      <c r="F46">
-        <v>34</v>
-      </c>
-      <c r="G46">
-        <v>36</v>
-      </c>
-      <c r="H46">
-        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1657,25 +1660,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D47">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E47">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F47">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G47">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H47">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1683,25 +1686,25 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C48">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D48">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E48">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F48">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="G48">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="H48">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1709,25 +1712,25 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D49">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E49">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F49">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G49">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="H49">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1735,25 +1738,25 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C50">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D50">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E50">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F50">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G50">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H50">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1761,25 +1764,25 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C51">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D51">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E51">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F51">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G51">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H51">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1787,25 +1790,25 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C52">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D52">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E52">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F52">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="G52">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="H52">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1813,25 +1816,25 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D53">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E53">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F53">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G53">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H53">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1839,25 +1842,25 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>16</v>
+      </c>
+      <c r="E54">
+        <v>17</v>
+      </c>
+      <c r="F54">
         <v>19</v>
       </c>
-      <c r="D54">
-        <v>31</v>
-      </c>
-      <c r="E54">
-        <v>35</v>
-      </c>
-      <c r="F54">
-        <v>36</v>
-      </c>
       <c r="G54">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H54">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1865,25 +1868,25 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C55">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D55">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E55">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F55">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G55">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H55">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1891,25 +1894,25 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C56">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D56">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E56">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F56">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G56">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H56">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1917,25 +1920,25 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C57">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D57">
+        <v>16</v>
+      </c>
+      <c r="E57">
+        <v>26</v>
+      </c>
+      <c r="F57">
         <v>30</v>
       </c>
-      <c r="E57">
-        <v>36</v>
-      </c>
-      <c r="F57">
-        <v>46</v>
-      </c>
       <c r="G57">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H57">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1943,25 +1946,25 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C58">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D58">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E58">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F58">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="G58">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H58">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -1969,24 +1972,50 @@
         <v>57</v>
       </c>
       <c r="B59">
+        <v>14</v>
+      </c>
+      <c r="C59">
+        <v>27</v>
+      </c>
+      <c r="D59">
+        <v>28</v>
+      </c>
+      <c r="E59">
+        <v>30</v>
+      </c>
+      <c r="F59">
+        <v>33</v>
+      </c>
+      <c r="G59">
+        <v>49</v>
+      </c>
+      <c r="H59">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60">
         <v>5</v>
       </c>
-      <c r="C59">
+      <c r="C60">
         <v>6</v>
       </c>
-      <c r="D59">
+      <c r="D60">
         <v>20</v>
       </c>
-      <c r="E59">
+      <c r="E60">
         <v>29</v>
       </c>
-      <c r="F59">
+      <c r="F60">
         <v>41</v>
       </c>
-      <c r="G59">
+      <c r="G60">
         <v>43</v>
       </c>
-      <c r="H59">
+      <c r="H60">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
20170716 - Commit and Push
</commit_message>
<xml_diff>
--- a/Lotto/lotto/lotto-past-draws-archive-2017.xlsx
+++ b/Lotto/lotto/lotto-past-draws-archive-2017.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Lotto</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Bonus Ball</t>
+  </si>
+  <si>
+    <t>15 July 2017</t>
   </si>
   <si>
     <t>12 July 2017</t>
@@ -547,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -594,25 +597,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D6">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E6">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F6">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -620,25 +623,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>31</v>
+      </c>
+      <c r="E7">
         <v>33</v>
       </c>
-      <c r="D7">
-        <v>36</v>
-      </c>
-      <c r="E7">
-        <v>38</v>
-      </c>
       <c r="F7">
+        <v>35</v>
+      </c>
+      <c r="G7">
         <v>40</v>
       </c>
-      <c r="G7">
-        <v>45</v>
-      </c>
       <c r="H7">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -646,25 +649,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D8">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E8">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F8">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -672,25 +675,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F9">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="G9">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="H9">
-        <v>48</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -698,25 +701,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>19</v>
+      </c>
+      <c r="F10">
         <v>25</v>
       </c>
-      <c r="E10">
-        <v>29</v>
-      </c>
-      <c r="F10">
-        <v>30</v>
-      </c>
       <c r="G10">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="H10">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -727,22 +730,22 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D11">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G11">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H11">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -750,25 +753,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E12">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F12">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="G12">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H12">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -776,25 +779,25 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D13">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E13">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F13">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G13">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H13">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -802,25 +805,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D14">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E14">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G14">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H14">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -828,25 +831,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E15">
+        <v>19</v>
+      </c>
+      <c r="F15">
+        <v>33</v>
+      </c>
+      <c r="G15">
+        <v>42</v>
+      </c>
+      <c r="H15">
         <v>27</v>
-      </c>
-      <c r="F15">
-        <v>42</v>
-      </c>
-      <c r="G15">
-        <v>47</v>
-      </c>
-      <c r="H15">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -854,25 +857,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D16">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16">
+        <v>27</v>
+      </c>
+      <c r="F16">
+        <v>42</v>
+      </c>
+      <c r="G16">
+        <v>47</v>
+      </c>
+      <c r="H16">
         <v>28</v>
-      </c>
-      <c r="F16">
-        <v>32</v>
-      </c>
-      <c r="G16">
-        <v>45</v>
-      </c>
-      <c r="H16">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -880,25 +883,25 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E17">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F17">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G17">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H17">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -906,25 +909,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D18">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E18">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F18">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G18">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -932,25 +935,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D19">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E19">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F19">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G19">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H19">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -958,25 +961,25 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E20">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F20">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G20">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="H20">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -987,22 +990,22 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D21">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E21">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F21">
         <v>30</v>
       </c>
       <c r="G21">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1010,25 +1013,25 @@
         <v>20</v>
       </c>
       <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
         <v>12</v>
       </c>
-      <c r="C22">
-        <v>25</v>
-      </c>
-      <c r="D22">
-        <v>27</v>
-      </c>
       <c r="E22">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F22">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G22">
         <v>41</v>
       </c>
       <c r="H22">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1036,25 +1039,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E23">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F23">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G23">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H23">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1062,25 +1065,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>22</v>
+      </c>
+      <c r="F24">
         <v>26</v>
       </c>
-      <c r="E24">
-        <v>41</v>
-      </c>
-      <c r="F24">
-        <v>43</v>
-      </c>
       <c r="G24">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H24">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1088,25 +1091,25 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D25">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E25">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F25">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G25">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H25">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1114,25 +1117,25 @@
         <v>24</v>
       </c>
       <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
         <v>9</v>
       </c>
-      <c r="C26">
-        <v>11</v>
-      </c>
-      <c r="D26">
-        <v>16</v>
-      </c>
       <c r="E26">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F26">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G26">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="H26">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1140,25 +1143,25 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D27">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E27">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F27">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G27">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H27">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1166,25 +1169,25 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D28">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E28">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F28">
+        <v>43</v>
+      </c>
+      <c r="G28">
         <v>47</v>
       </c>
-      <c r="G28">
-        <v>48</v>
-      </c>
       <c r="H28">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1192,25 +1195,25 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D29">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E29">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F29">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G29">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H29">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1218,22 +1221,22 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D30">
+        <v>23</v>
+      </c>
+      <c r="E30">
         <v>26</v>
       </c>
-      <c r="E30">
-        <v>35</v>
-      </c>
       <c r="F30">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G30">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H30">
         <v>22</v>
@@ -1244,25 +1247,25 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D31">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E31">
         <v>35</v>
       </c>
       <c r="F31">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G31">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H31">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1270,25 +1273,25 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C32">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D32">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E32">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F32">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G32">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="H32">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1296,25 +1299,25 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D33">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E33">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F33">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G33">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1322,25 +1325,25 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C34">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D34">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E34">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F34">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G34">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H34">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1348,25 +1351,25 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C35">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D35">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E35">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F35">
         <v>35</v>
       </c>
       <c r="G35">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1374,25 +1377,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E36">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F36">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G36">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="H36">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1400,25 +1403,25 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D37">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E37">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F37">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G37">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H37">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1426,25 +1429,25 @@
         <v>36</v>
       </c>
       <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
         <v>5</v>
       </c>
-      <c r="C38">
-        <v>7</v>
-      </c>
       <c r="D38">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>19</v>
+      </c>
+      <c r="F38">
+        <v>24</v>
+      </c>
+      <c r="G38">
+        <v>25</v>
+      </c>
+      <c r="H38">
         <v>17</v>
-      </c>
-      <c r="E38">
-        <v>22</v>
-      </c>
-      <c r="F38">
-        <v>25</v>
-      </c>
-      <c r="G38">
-        <v>35</v>
-      </c>
-      <c r="H38">
-        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1452,25 +1455,25 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E39">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F39">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G39">
+        <v>35</v>
+      </c>
+      <c r="H39">
         <v>49</v>
-      </c>
-      <c r="H39">
-        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1478,25 +1481,25 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>7</v>
+      </c>
+      <c r="E40">
         <v>13</v>
       </c>
-      <c r="D40">
-        <v>14</v>
-      </c>
-      <c r="E40">
-        <v>25</v>
-      </c>
       <c r="F40">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="G40">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="H40">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1504,25 +1507,25 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D41">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E41">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F41">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G41">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1530,25 +1533,25 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C42">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D42">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E42">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F42">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G42">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H42">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1556,25 +1559,25 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D43">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E43">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F43">
         <v>38</v>
       </c>
       <c r="G43">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H43">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1582,25 +1585,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D44">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E44">
+        <v>31</v>
+      </c>
+      <c r="F44">
+        <v>38</v>
+      </c>
+      <c r="G44">
         <v>41</v>
       </c>
-      <c r="F44">
-        <v>43</v>
-      </c>
-      <c r="G44">
-        <v>44</v>
-      </c>
       <c r="H44">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1608,25 +1611,25 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C45">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D45">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="E45">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F45">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G45">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H45">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1637,22 +1640,22 @@
         <v>7</v>
       </c>
       <c r="C46">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D46">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E46">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F46">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G46">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H46">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1660,25 +1663,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C47">
+        <v>12</v>
+      </c>
+      <c r="D47">
+        <v>16</v>
+      </c>
+      <c r="E47">
+        <v>39</v>
+      </c>
+      <c r="F47">
+        <v>46</v>
+      </c>
+      <c r="G47">
+        <v>48</v>
+      </c>
+      <c r="H47">
         <v>14</v>
-      </c>
-      <c r="D47">
-        <v>19</v>
-      </c>
-      <c r="E47">
-        <v>31</v>
-      </c>
-      <c r="F47">
-        <v>34</v>
-      </c>
-      <c r="G47">
-        <v>36</v>
-      </c>
-      <c r="H47">
-        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1686,25 +1689,25 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D48">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E48">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F48">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G48">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H48">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1712,25 +1715,25 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C49">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D49">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E49">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F49">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="G49">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="H49">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1738,25 +1741,25 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D50">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E50">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F50">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G50">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="H50">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1764,25 +1767,25 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C51">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D51">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E51">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F51">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G51">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H51">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1790,25 +1793,25 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C52">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D52">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E52">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F52">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G52">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H52">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1816,25 +1819,25 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C53">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D53">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E53">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F53">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="G53">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="H53">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1842,25 +1845,25 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D54">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E54">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F54">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G54">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H54">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1868,25 +1871,25 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>16</v>
+      </c>
+      <c r="E55">
+        <v>17</v>
+      </c>
+      <c r="F55">
         <v>19</v>
       </c>
-      <c r="D55">
-        <v>31</v>
-      </c>
-      <c r="E55">
-        <v>35</v>
-      </c>
-      <c r="F55">
-        <v>36</v>
-      </c>
       <c r="G55">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H55">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1894,25 +1897,25 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C56">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D56">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E56">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F56">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G56">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H56">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1920,25 +1923,25 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C57">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D57">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E57">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F57">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G57">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H57">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1946,25 +1949,25 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D58">
+        <v>16</v>
+      </c>
+      <c r="E58">
+        <v>26</v>
+      </c>
+      <c r="F58">
         <v>30</v>
       </c>
-      <c r="E58">
-        <v>36</v>
-      </c>
-      <c r="F58">
-        <v>46</v>
-      </c>
       <c r="G58">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H58">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -1972,25 +1975,25 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C59">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D59">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E59">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F59">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="G59">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H59">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -1998,24 +2001,50 @@
         <v>58</v>
       </c>
       <c r="B60">
+        <v>14</v>
+      </c>
+      <c r="C60">
+        <v>27</v>
+      </c>
+      <c r="D60">
+        <v>28</v>
+      </c>
+      <c r="E60">
+        <v>30</v>
+      </c>
+      <c r="F60">
+        <v>33</v>
+      </c>
+      <c r="G60">
+        <v>49</v>
+      </c>
+      <c r="H60">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61">
         <v>5</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>6</v>
       </c>
-      <c r="D60">
+      <c r="D61">
         <v>20</v>
       </c>
-      <c r="E60">
+      <c r="E61">
         <v>29</v>
       </c>
-      <c r="F60">
+      <c r="F61">
         <v>41</v>
       </c>
-      <c r="G60">
+      <c r="G61">
         <v>43</v>
       </c>
-      <c r="H60">
+      <c r="H61">
         <v>15</v>
       </c>
     </row>

</xml_diff>